<commit_message>
Update to match updated logs
</commit_message>
<xml_diff>
--- a/04-Development-and-Quality-Assurance/Evaluation-Testing/Logs/Compare Data.xlsx
+++ b/04-Development-and-Quality-Assurance/Evaluation-Testing/Logs/Compare Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://autuni-my.sharepoint.com/personal/cgr2690_autuni_ac_nz/Documents/Data/COMP703/Linux Networking/04-Development-and-Quality-Assurance/Logs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://autuni-my.sharepoint.com/personal/cgr2690_autuni_ac_nz/Documents/Data/COMP703/Linux Networking/04-Development-and-Quality-Assurance/Evaluation-Testing/Logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="282" documentId="8_{9B9BE8A9-2D06-4744-8A91-5D8CADA897AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17F63A68-44DE-4CE0-BED3-B220D636DBA4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{BE2AF4ED-48B1-4187-9EDF-7287B39E53F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{BE2AF4ED-48B1-4187-9EDF-7287B39E53F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -70,6 +70,30 @@
     <t>Packet Size</t>
   </si>
   <si>
+    <t>IPv4 TCP Average Delay</t>
+  </si>
+  <si>
+    <t>IPv4 TCP Jitter</t>
+  </si>
+  <si>
+    <t>IPv4 TCP Bitrate</t>
+  </si>
+  <si>
+    <t>IPv4 TCP Packet Loss</t>
+  </si>
+  <si>
+    <t>IPv4 UDP Average Delay</t>
+  </si>
+  <si>
+    <t>IPv4 UDP Jitter</t>
+  </si>
+  <si>
+    <t>IPv4 UDP Bitrate</t>
+  </si>
+  <si>
+    <t>IPv4 UDP Packet Loss</t>
+  </si>
+  <si>
     <t>TCP Average Delay</t>
   </si>
   <si>
@@ -94,28 +118,31 @@
     <t>UDP Packet Loss</t>
   </si>
   <si>
-    <t>IPv4 TCP Average Delay</t>
+    <t>Ubuntu Run 3 (Latest)</t>
   </si>
   <si>
-    <t>IPv4 TCP Jitter</t>
+    <t xml:space="preserve">Kali </t>
   </si>
   <si>
-    <t>IPv4 TCP Bitrate</t>
+    <t xml:space="preserve">Fedora </t>
   </si>
   <si>
-    <t>IPv4 TCP Packet Loss</t>
+    <t>Delay</t>
   </si>
   <si>
-    <t>IPv4 UDP Average Delay</t>
+    <t>Jitter</t>
   </si>
   <si>
-    <t>IPv4 UDP Jitter</t>
+    <t>Bitrate</t>
   </si>
   <si>
-    <t>IPv4 UDP Bitrate</t>
+    <t>Packet Loss</t>
   </si>
   <si>
-    <t>IPv4 UDP Packet Loss</t>
+    <t>Ubuntu IPv4 TCP Average Delay</t>
+  </si>
+  <si>
+    <t>Ubuntu IPv4 UDP Average Delay</t>
   </si>
   <si>
     <t>Fedora IPv4 TCP Average Delay</t>
@@ -130,6 +157,12 @@
     <t>Kali IPv4 UDP Average Delay</t>
   </si>
   <si>
+    <t>Ubuntu IPv4 TCP Jitter</t>
+  </si>
+  <si>
+    <t>Ubuntu IPv4 UDP Jitter</t>
+  </si>
+  <si>
     <t>Fedora IPv4 TCP Jitter</t>
   </si>
   <si>
@@ -142,10 +175,10 @@
     <t>Kali IPv4 UDP Jitter</t>
   </si>
   <si>
-    <t xml:space="preserve">Kali </t>
+    <t>Ubuntu IPv4 TCP Bitrate</t>
   </si>
   <si>
-    <t xml:space="preserve">Fedora </t>
+    <t>Ubuntu IPv4 UDP Bitrate</t>
   </si>
   <si>
     <t>Fedora IPv4 TCP Bitrate</t>
@@ -160,6 +193,12 @@
     <t>Kali IPv4 UDP Bitrate</t>
   </si>
   <si>
+    <t>Ubuntu IPv4 TCP Packet Loss</t>
+  </si>
+  <si>
+    <t>Ubuntu IPv4 UDP Packet Loss</t>
+  </si>
+  <si>
     <t>Fedora IPv4 TCP Packet Loss</t>
   </si>
   <si>
@@ -170,24 +209,6 @@
   </si>
   <si>
     <t>Kali IPv4 UDP Packet Loss</t>
-  </si>
-  <si>
-    <t>Ubuntu IPv4 UDP Average Delay</t>
-  </si>
-  <si>
-    <t>Ubuntu IPv4 TCP Average Delay</t>
-  </si>
-  <si>
-    <t>Ubuntu IPv4 TCP Packet Loss</t>
-  </si>
-  <si>
-    <t>Ubuntu IPv4 UDP Packet Loss</t>
-  </si>
-  <si>
-    <t>Ubuntu IPv4 TCP Bitrate</t>
-  </si>
-  <si>
-    <t>Ubuntu IPv4 UDP Bitrate</t>
   </si>
   <si>
     <t>Ubuntu IPv6 TCP Average Delay</t>
@@ -206,6 +227,12 @@
   </si>
   <si>
     <t>Kali IPv6 UDP Average Delay</t>
+  </si>
+  <si>
+    <t>Ubuntu IPv6 TCP Jitter</t>
+  </si>
+  <si>
+    <t>Ubuntu IPv6 UDP  Jitter</t>
   </si>
   <si>
     <t>Fedora IPv6 TCP Jitter</t>
@@ -256,34 +283,7 @@
     <t>Kali IPv6 UDP Packet Loss</t>
   </si>
   <si>
-    <t>Ubuntu IPv6 UDP  Jitter</t>
-  </si>
-  <si>
-    <t>Ubuntu IPv6 TCP Jitter</t>
-  </si>
-  <si>
-    <t>Ubuntu IPv4 TCP Jitter</t>
-  </si>
-  <si>
-    <t>Ubuntu IPv4 UDP Jitter</t>
-  </si>
-  <si>
-    <t>Delay</t>
-  </si>
-  <si>
-    <t>Jitter</t>
-  </si>
-  <si>
-    <t>Bitrate</t>
-  </si>
-  <si>
-    <t>Packet Loss</t>
-  </si>
-  <si>
     <t>Ubuntu Run 3</t>
-  </si>
-  <si>
-    <t>Ubuntu Run 3 (Latest)</t>
   </si>
 </sst>
 </file>
@@ -26731,7 +26731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75707BDC-D342-4112-9D19-1697BB5EC01E}">
   <dimension ref="B1:AH139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AB128" sqref="AB128:AB139"/>
     </sheetView>
   </sheetViews>
@@ -26846,61 +26846,61 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
         <v>8</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="L7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="S7" t="s">
         <v>8</v>
       </c>
       <c r="T7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="U7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="V7" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="W7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="Y7" t="s">
         <v>8</v>
       </c>
       <c r="Z7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="AA7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="AB7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AC7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.25">
@@ -27756,61 +27756,61 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H26" t="s">
         <v>8</v>
       </c>
       <c r="I26" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="J26" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K26" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="L26" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="S26" t="s">
         <v>8</v>
       </c>
       <c r="T26" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="U26" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="V26" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="W26" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="Y26" t="s">
         <v>8</v>
       </c>
       <c r="Z26" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="AA26" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="AB26" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AC26" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.25">
@@ -28560,7 +28560,7 @@
     <row r="39" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -28633,7 +28633,7 @@
     </row>
     <row r="43" spans="2:34" x14ac:dyDescent="0.25">
       <c r="AH43" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="2:34" x14ac:dyDescent="0.25">
@@ -28666,7 +28666,7 @@
       <c r="AB44" s="5"/>
       <c r="AC44" s="5"/>
       <c r="AH44" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="2:34" x14ac:dyDescent="0.25">
@@ -28674,61 +28674,61 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F45" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H45" t="s">
         <v>8</v>
       </c>
       <c r="I45" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="J45" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K45" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="L45" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="S45" t="s">
         <v>8</v>
       </c>
       <c r="T45" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="U45" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="V45" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="W45" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="Y45" t="s">
         <v>8</v>
       </c>
       <c r="Z45" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="AA45" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="AB45" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AC45" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="2:34" x14ac:dyDescent="0.25">
@@ -29546,7 +29546,7 @@
     </row>
     <row r="76" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B76" s="5" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -29555,7 +29555,7 @@
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
       <c r="J76" s="5" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
@@ -29564,7 +29564,7 @@
       <c r="O76" s="5"/>
       <c r="P76" s="5"/>
       <c r="R76" s="5" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="S76" s="5"/>
       <c r="T76" s="5"/>
@@ -29573,7 +29573,7 @@
       <c r="W76" s="5"/>
       <c r="X76" s="5"/>
       <c r="Z76" s="5" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="AA76" s="5"/>
       <c r="AB76" s="5"/>
@@ -29587,85 +29587,85 @@
         <v>8</v>
       </c>
       <c r="C77" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D77" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E77" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F77" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="G77" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="H77" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="J77" t="s">
         <v>8</v>
       </c>
       <c r="K77" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="L77" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="M77" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="N77" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="O77" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="P77" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="R77" t="s">
         <v>8</v>
       </c>
       <c r="S77" t="s">
+        <v>44</v>
+      </c>
+      <c r="T77" t="s">
+        <v>45</v>
+      </c>
+      <c r="U77" t="s">
+        <v>46</v>
+      </c>
+      <c r="V77" t="s">
         <v>47</v>
       </c>
-      <c r="T77" t="s">
+      <c r="W77" t="s">
         <v>48</v>
       </c>
-      <c r="U77" t="s">
-        <v>35</v>
-      </c>
-      <c r="V77" t="s">
-        <v>36</v>
-      </c>
-      <c r="W77" t="s">
-        <v>37</v>
-      </c>
       <c r="X77" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="Z77" t="s">
         <v>8</v>
       </c>
       <c r="AA77" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="AB77" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="AC77" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="AD77" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="AE77" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="AF77" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="78" spans="2:32" x14ac:dyDescent="0.25">
@@ -30738,7 +30738,7 @@
     </row>
     <row r="126" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B126" s="5" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
@@ -30747,7 +30747,7 @@
       <c r="G126" s="5"/>
       <c r="H126" s="5"/>
       <c r="J126" s="5" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="K126" s="5"/>
       <c r="L126" s="5"/>
@@ -30756,7 +30756,7 @@
       <c r="O126" s="5"/>
       <c r="P126" s="5"/>
       <c r="R126" s="5" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="S126" s="5"/>
       <c r="T126" s="5"/>
@@ -30765,7 +30765,7 @@
       <c r="W126" s="5"/>
       <c r="X126" s="5"/>
       <c r="Z126" s="5" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="AA126" s="5"/>
       <c r="AB126" s="5"/>
@@ -30779,85 +30779,85 @@
         <v>8</v>
       </c>
       <c r="C127" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D127" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E127" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F127" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G127" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H127" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="J127" t="s">
         <v>8</v>
       </c>
       <c r="K127" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="L127" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="M127" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="N127" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="O127" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="P127" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="R127" t="s">
         <v>8</v>
       </c>
       <c r="S127" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="T127" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="U127" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="V127" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="W127" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="X127" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="Z127" t="s">
         <v>8</v>
       </c>
       <c r="AA127" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="AB127" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="AC127" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="AD127" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="AE127" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="AF127" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="128" spans="2:32" x14ac:dyDescent="0.25">
@@ -31945,7 +31945,7 @@
     <row r="1" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -32051,61 +32051,61 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
         <v>8</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="L7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="S7" t="s">
         <v>8</v>
       </c>
       <c r="T7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="U7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="V7" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="W7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="Y7" t="s">
         <v>8</v>
       </c>
       <c r="Z7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="AA7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="AB7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AC7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.25">

</xml_diff>